<commit_message>
film inspection & PDF imroved
</commit_message>
<xml_diff>
--- a/backend/templates/UC-16gsm-165W.xlsx
+++ b/backend/templates/UC-16gsm-165W.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2A418A-AA7C-4C2E-9003-2C1AAB0969BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6437AD22-BEE0-402A-90C3-2540BC52E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,21 +899,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1348,25 +1333,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="284">
+  <cellXfs count="294">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1382,61 +1378,61 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1445,7 +1441,7 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1454,13 +1450,13 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1527,150 +1523,150 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1694,13 +1690,13 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1712,7 +1708,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1748,30 +1744,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1799,7 +1795,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1807,7 +1803,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1815,20 +1811,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1838,7 +1834,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1847,6 +1843,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1862,7 +1867,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1883,46 +1888,46 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1937,110 +1942,107 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2048,28 +2050,25 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2081,40 +2080,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2126,64 +2125,64 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2204,11 +2203,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2216,30 +2218,27 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2247,6 +2246,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2807,7 +2833,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,31 +2847,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
       <c r="I1" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
       <c r="I2" s="55" t="s">
         <v>22</v>
       </c>
@@ -2867,8 +2893,8 @@
       <c r="A4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="175"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="178"/>
       <c r="D4" s="60" t="s">
         <v>3</v>
       </c>
@@ -2889,8 +2915,8 @@
       <c r="A5" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="176"/>
-      <c r="C5" s="177"/>
+      <c r="B5" s="179"/>
+      <c r="C5" s="180"/>
       <c r="D5" s="63" t="s">
         <v>6</v>
       </c>
@@ -2905,46 +2931,46 @@
       <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="159" t="s">
+      <c r="A6" s="162" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="160"/>
-      <c r="C6" s="161"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="164"/>
       <c r="D6" s="148"/>
       <c r="E6" s="146"/>
       <c r="F6" s="146"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="153"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="156"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="162" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="154"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154" t="s">
+      <c r="A7" s="165" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="157"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="156" t="s">
+      <c r="E7" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="156" t="s">
+      <c r="F7" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="154" t="s">
+      <c r="G7" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="154"/>
-      <c r="I7" s="155"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="158"/>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="163"/>
-      <c r="B8" s="164"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
+      <c r="A8" s="166"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="167"/>
+      <c r="D8" s="167"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
       <c r="G8" s="65" t="s">
         <v>37</v>
       </c>
@@ -3286,12 +3312,12 @@
       <c r="I38" s="94"/>
     </row>
     <row r="39" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="169" t="s">
+      <c r="A39" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="170"/>
-      <c r="C39" s="170"/>
-      <c r="D39" s="18" t="e">
+      <c r="B39" s="169"/>
+      <c r="C39" s="291"/>
+      <c r="D39" s="150" t="e">
         <f>AVERAGE(D9:D38)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3317,12 +3343,12 @@
       </c>
     </row>
     <row r="40" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="167" t="s">
+      <c r="A40" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="168"/>
-      <c r="C40" s="168"/>
-      <c r="D40" s="25">
+      <c r="B40" s="171"/>
+      <c r="C40" s="292"/>
+      <c r="D40" s="151">
         <f>MIN(D9:D38)</f>
         <v>0</v>
       </c>
@@ -3348,12 +3374,12 @@
       </c>
     </row>
     <row r="41" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="165" t="s">
+      <c r="A41" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="166"/>
-      <c r="C41" s="166"/>
-      <c r="D41" s="96">
+      <c r="B41" s="173"/>
+      <c r="C41" s="293"/>
+      <c r="D41" s="152">
         <f>MAX(D9:D38)</f>
         <v>0</v>
       </c>
@@ -3385,8 +3411,8 @@
       <c r="A42" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="172"/>
-      <c r="C42" s="172"/>
+      <c r="B42" s="175"/>
+      <c r="C42" s="175"/>
       <c r="D42" s="98" t="s">
         <v>16</v>
       </c>
@@ -3402,8 +3428,8 @@
     </row>
     <row r="43" spans="1:12" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="102"/>
-      <c r="B43" s="173"/>
-      <c r="C43" s="173"/>
+      <c r="B43" s="176"/>
+      <c r="C43" s="176"/>
       <c r="D43" s="98"/>
       <c r="E43" s="99"/>
       <c r="F43" s="100"/>
@@ -3412,11 +3438,11 @@
       <c r="I43" s="101"/>
     </row>
     <row r="44" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="158" t="s">
+      <c r="A44" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="158"/>
-      <c r="C44" s="158"/>
+      <c r="B44" s="161"/>
+      <c r="C44" s="161"/>
       <c r="D44" s="103"/>
       <c r="E44" s="104" t="s">
         <v>109</v>
@@ -3429,19 +3455,19 @@
       <c r="I44" s="57"/>
     </row>
     <row r="45" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="158" t="s">
+      <c r="A45" s="161" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="158"/>
-      <c r="C45" s="158"/>
+      <c r="B45" s="161"/>
+      <c r="C45" s="161"/>
       <c r="D45" s="103"/>
       <c r="E45" s="57"/>
       <c r="F45" s="57"/>
       <c r="G45" s="57"/>
-      <c r="H45" s="150" t="s">
+      <c r="H45" s="153" t="s">
         <v>26</v>
       </c>
-      <c r="I45" s="150"/>
+      <c r="I45" s="153"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="44"/>
@@ -3473,9 +3499,9 @@
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E38">
     <cfRule type="cellIs" dxfId="14" priority="5" operator="notBetween">
@@ -3519,7 +3545,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,31 +3556,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
       <c r="I1" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
       <c r="I2" s="55" t="s">
         <v>22</v>
       </c>
@@ -3579,11 +3605,11 @@
       <c r="A4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="174">
+      <c r="B4" s="177">
         <f>Page1!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="178"/>
       <c r="D4" s="60" t="s">
         <v>3</v>
       </c>
@@ -3613,11 +3639,11 @@
       <c r="A5" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="191">
+      <c r="B5" s="195">
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="192"/>
+      <c r="C5" s="196"/>
       <c r="D5" s="106" t="s">
         <v>6</v>
       </c>
@@ -3641,83 +3667,83 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="49" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="201" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="198"/>
-      <c r="C6" s="198"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="199"/>
+      <c r="B6" s="202"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="203"/>
       <c r="G6" s="108"/>
       <c r="H6" s="109"/>
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="182" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="183"/>
-      <c r="C7" s="184"/>
-      <c r="D7" s="200" t="s">
+      <c r="A7" s="185" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="186"/>
+      <c r="C7" s="187"/>
+      <c r="D7" s="204" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="201"/>
-      <c r="F7" s="202"/>
-      <c r="G7" s="188" t="s">
+      <c r="E7" s="205"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="191" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="180" t="s">
+      <c r="I7" s="183" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="182"/>
-      <c r="B8" s="183"/>
-      <c r="C8" s="184"/>
-      <c r="D8" s="193" t="s">
+      <c r="A8" s="185"/>
+      <c r="B8" s="186"/>
+      <c r="C8" s="187"/>
+      <c r="D8" s="197" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="196" t="s">
+      <c r="E8" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="192" t="s">
+      <c r="F8" s="196" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="188"/>
+      <c r="G8" s="191"/>
       <c r="H8" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="I8" s="180"/>
+      <c r="I8" s="183"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="182"/>
-      <c r="B9" s="183"/>
-      <c r="C9" s="184"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="196"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="188"/>
+      <c r="A9" s="185"/>
+      <c r="B9" s="186"/>
+      <c r="C9" s="187"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="187"/>
+      <c r="G9" s="191"/>
       <c r="H9" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="I9" s="180"/>
+      <c r="I9" s="183"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="185"/>
-      <c r="B10" s="186"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="164"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="157"/>
+      <c r="A10" s="188"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="199"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="190"/>
+      <c r="G10" s="160"/>
       <c r="H10" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="181"/>
+      <c r="I10" s="184"/>
     </row>
     <row r="11" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="111"/>
@@ -4194,12 +4220,12 @@
       </c>
     </row>
     <row r="41" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="169" t="s">
+      <c r="A41" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="170"/>
-      <c r="C41" s="170"/>
-      <c r="D41" s="18" t="e">
+      <c r="B41" s="169"/>
+      <c r="C41" s="291"/>
+      <c r="D41" s="150" t="e">
         <f>AVERAGE(D11:D40)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4225,12 +4251,12 @@
       </c>
     </row>
     <row r="42" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="167" t="s">
+      <c r="A42" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="168"/>
-      <c r="C42" s="168"/>
-      <c r="D42" s="25">
+      <c r="B42" s="171"/>
+      <c r="C42" s="292"/>
+      <c r="D42" s="151">
         <f>MIN(D11:D40)</f>
         <v>0</v>
       </c>
@@ -4256,12 +4282,12 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="165" t="s">
+      <c r="A43" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="166"/>
-      <c r="C43" s="166"/>
-      <c r="D43" s="96">
+      <c r="B43" s="173"/>
+      <c r="C43" s="293"/>
+      <c r="D43" s="152">
         <f>MAX(D11:D40)</f>
         <v>0</v>
       </c>
@@ -4290,11 +4316,11 @@
       <c r="A44" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="172">
+      <c r="B44" s="192">
         <f>Page1!B42</f>
         <v>0</v>
       </c>
-      <c r="C44" s="189"/>
+      <c r="C44" s="193"/>
       <c r="D44" s="128" t="s">
         <v>16</v>
       </c>
@@ -4313,11 +4339,11 @@
     </row>
     <row r="45" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="132"/>
-      <c r="B45" s="173">
+      <c r="B45" s="176">
         <f>Page1!B43</f>
         <v>0</v>
       </c>
-      <c r="C45" s="190"/>
+      <c r="C45" s="194"/>
       <c r="D45" s="128"/>
       <c r="E45" s="128"/>
       <c r="F45" s="129"/>
@@ -4329,11 +4355,11 @@
       <c r="I45" s="131"/>
     </row>
     <row r="46" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="178" t="s">
+      <c r="A46" s="181" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="178"/>
-      <c r="C46" s="178"/>
+      <c r="B46" s="181"/>
+      <c r="C46" s="181"/>
       <c r="D46" s="133"/>
       <c r="E46" s="134" t="s">
         <v>109</v>
@@ -4347,19 +4373,19 @@
       <c r="I46" s="133"/>
     </row>
     <row r="47" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="178" t="s">
+      <c r="A47" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="178"/>
-      <c r="C47" s="178"/>
+      <c r="B47" s="181"/>
+      <c r="C47" s="181"/>
       <c r="D47" s="133"/>
       <c r="E47" s="133"/>
       <c r="F47" s="133"/>
       <c r="G47" s="133"/>
-      <c r="H47" s="179" t="s">
+      <c r="H47" s="182" t="s">
         <v>27</v>
       </c>
-      <c r="I47" s="179"/>
+      <c r="I47" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -4379,11 +4405,11 @@
     <mergeCell ref="A7:C10"/>
     <mergeCell ref="G7:G10"/>
     <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A42:C42"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <conditionalFormatting sqref="D11:D40">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="notBetween">
@@ -4433,7 +4459,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,31 +4470,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
       <c r="I1" s="54" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="171"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
       <c r="I2" s="55" t="s">
         <v>22</v>
       </c>
@@ -4493,11 +4519,11 @@
       <c r="A4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="174">
+      <c r="B4" s="177">
         <f>Page1!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="175"/>
+      <c r="C4" s="178"/>
       <c r="D4" s="60" t="s">
         <v>3</v>
       </c>
@@ -4527,11 +4553,11 @@
       <c r="A5" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="191">
+      <c r="B5" s="195">
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="192"/>
+      <c r="C5" s="196"/>
       <c r="D5" s="106" t="s">
         <v>6</v>
       </c>
@@ -4555,49 +4581,49 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="49" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="201" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="198"/>
-      <c r="C6" s="151"/>
-      <c r="D6" s="203"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="204"/>
-      <c r="I6" s="205"/>
+      <c r="B6" s="202"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="156"/>
+      <c r="H6" s="207"/>
+      <c r="I6" s="208"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="208" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="204"/>
-      <c r="C7" s="204"/>
-      <c r="D7" s="209" t="s">
+      <c r="A7" s="211" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="207"/>
+      <c r="C7" s="287"/>
+      <c r="D7" s="285" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="211" t="s">
+      <c r="E7" s="212" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="211" t="s">
+      <c r="F7" s="212" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="213" t="s">
+      <c r="G7" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="183"/>
-      <c r="I7" s="206"/>
+      <c r="H7" s="186"/>
+      <c r="I7" s="209"/>
     </row>
     <row r="8" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="185"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="210"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="212"/>
-      <c r="G8" s="214"/>
-      <c r="H8" s="183"/>
-      <c r="I8" s="206"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="189"/>
+      <c r="C8" s="190"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="213"/>
+      <c r="F8" s="213"/>
+      <c r="G8" s="215"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="209"/>
     </row>
     <row r="9" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="111"/>
@@ -4607,8 +4633,8 @@
       <c r="E9" s="84"/>
       <c r="F9" s="84"/>
       <c r="G9" s="136"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="206"/>
+      <c r="H9" s="186"/>
+      <c r="I9" s="209"/>
     </row>
     <row r="10" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="73"/>
@@ -4618,8 +4644,8 @@
       <c r="E10" s="79"/>
       <c r="F10" s="79"/>
       <c r="G10" s="138"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="206"/>
+      <c r="H10" s="186"/>
+      <c r="I10" s="209"/>
     </row>
     <row r="11" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="73"/>
@@ -4629,8 +4655,8 @@
       <c r="E11" s="79"/>
       <c r="F11" s="79"/>
       <c r="G11" s="138"/>
-      <c r="H11" s="183"/>
-      <c r="I11" s="206"/>
+      <c r="H11" s="186"/>
+      <c r="I11" s="209"/>
     </row>
     <row r="12" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="73"/>
@@ -4640,8 +4666,8 @@
       <c r="E12" s="79"/>
       <c r="F12" s="79"/>
       <c r="G12" s="138"/>
-      <c r="H12" s="183"/>
-      <c r="I12" s="206"/>
+      <c r="H12" s="186"/>
+      <c r="I12" s="209"/>
     </row>
     <row r="13" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="73"/>
@@ -4651,8 +4677,8 @@
       <c r="E13" s="79"/>
       <c r="F13" s="79"/>
       <c r="G13" s="138"/>
-      <c r="H13" s="183"/>
-      <c r="I13" s="206"/>
+      <c r="H13" s="186"/>
+      <c r="I13" s="209"/>
     </row>
     <row r="14" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="73"/>
@@ -4662,8 +4688,8 @@
       <c r="E14" s="79"/>
       <c r="F14" s="79"/>
       <c r="G14" s="138"/>
-      <c r="H14" s="183"/>
-      <c r="I14" s="206"/>
+      <c r="H14" s="186"/>
+      <c r="I14" s="209"/>
     </row>
     <row r="15" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="73"/>
@@ -4673,8 +4699,8 @@
       <c r="E15" s="79"/>
       <c r="F15" s="79"/>
       <c r="G15" s="138"/>
-      <c r="H15" s="183"/>
-      <c r="I15" s="206"/>
+      <c r="H15" s="186"/>
+      <c r="I15" s="209"/>
     </row>
     <row r="16" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="73"/>
@@ -4684,8 +4710,8 @@
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
       <c r="G16" s="138"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="206"/>
+      <c r="H16" s="186"/>
+      <c r="I16" s="209"/>
     </row>
     <row r="17" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73"/>
@@ -4695,8 +4721,8 @@
       <c r="E17" s="79"/>
       <c r="F17" s="79"/>
       <c r="G17" s="138"/>
-      <c r="H17" s="183"/>
-      <c r="I17" s="206"/>
+      <c r="H17" s="186"/>
+      <c r="I17" s="209"/>
     </row>
     <row r="18" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="73"/>
@@ -4706,8 +4732,8 @@
       <c r="E18" s="79"/>
       <c r="F18" s="79"/>
       <c r="G18" s="138"/>
-      <c r="H18" s="183"/>
-      <c r="I18" s="206"/>
+      <c r="H18" s="186"/>
+      <c r="I18" s="209"/>
     </row>
     <row r="19" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="73"/>
@@ -4717,8 +4743,8 @@
       <c r="E19" s="79"/>
       <c r="F19" s="79"/>
       <c r="G19" s="138"/>
-      <c r="H19" s="183"/>
-      <c r="I19" s="206"/>
+      <c r="H19" s="186"/>
+      <c r="I19" s="209"/>
     </row>
     <row r="20" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="73"/>
@@ -4728,8 +4754,8 @@
       <c r="E20" s="79"/>
       <c r="F20" s="79"/>
       <c r="G20" s="138"/>
-      <c r="H20" s="183"/>
-      <c r="I20" s="206"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="209"/>
     </row>
     <row r="21" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="73"/>
@@ -4739,8 +4765,8 @@
       <c r="E21" s="79"/>
       <c r="F21" s="79"/>
       <c r="G21" s="138"/>
-      <c r="H21" s="183"/>
-      <c r="I21" s="206"/>
+      <c r="H21" s="186"/>
+      <c r="I21" s="209"/>
     </row>
     <row r="22" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="73"/>
@@ -4750,8 +4776,8 @@
       <c r="E22" s="79"/>
       <c r="F22" s="79"/>
       <c r="G22" s="138"/>
-      <c r="H22" s="183"/>
-      <c r="I22" s="206"/>
+      <c r="H22" s="186"/>
+      <c r="I22" s="209"/>
     </row>
     <row r="23" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="73"/>
@@ -4761,8 +4787,8 @@
       <c r="E23" s="79"/>
       <c r="F23" s="79"/>
       <c r="G23" s="138"/>
-      <c r="H23" s="183"/>
-      <c r="I23" s="206"/>
+      <c r="H23" s="186"/>
+      <c r="I23" s="209"/>
     </row>
     <row r="24" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="73"/>
@@ -4772,8 +4798,8 @@
       <c r="E24" s="84"/>
       <c r="F24" s="84"/>
       <c r="G24" s="136"/>
-      <c r="H24" s="183"/>
-      <c r="I24" s="206"/>
+      <c r="H24" s="186"/>
+      <c r="I24" s="209"/>
     </row>
     <row r="25" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="73"/>
@@ -4783,8 +4809,8 @@
       <c r="E25" s="79"/>
       <c r="F25" s="79"/>
       <c r="G25" s="138"/>
-      <c r="H25" s="183"/>
-      <c r="I25" s="206"/>
+      <c r="H25" s="186"/>
+      <c r="I25" s="209"/>
     </row>
     <row r="26" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="73"/>
@@ -4794,8 +4820,8 @@
       <c r="E26" s="79"/>
       <c r="F26" s="79"/>
       <c r="G26" s="138"/>
-      <c r="H26" s="183"/>
-      <c r="I26" s="206"/>
+      <c r="H26" s="186"/>
+      <c r="I26" s="209"/>
     </row>
     <row r="27" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="73"/>
@@ -4805,8 +4831,8 @@
       <c r="E27" s="79"/>
       <c r="F27" s="79"/>
       <c r="G27" s="138"/>
-      <c r="H27" s="183"/>
-      <c r="I27" s="206"/>
+      <c r="H27" s="186"/>
+      <c r="I27" s="209"/>
     </row>
     <row r="28" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
@@ -4816,8 +4842,8 @@
       <c r="E28" s="79"/>
       <c r="F28" s="79"/>
       <c r="G28" s="138"/>
-      <c r="H28" s="183"/>
-      <c r="I28" s="206"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="209"/>
     </row>
     <row r="29" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="73"/>
@@ -4827,8 +4853,8 @@
       <c r="E29" s="79"/>
       <c r="F29" s="79"/>
       <c r="G29" s="138"/>
-      <c r="H29" s="183"/>
-      <c r="I29" s="206"/>
+      <c r="H29" s="186"/>
+      <c r="I29" s="209"/>
     </row>
     <row r="30" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="73"/>
@@ -4838,8 +4864,8 @@
       <c r="E30" s="79"/>
       <c r="F30" s="79"/>
       <c r="G30" s="138"/>
-      <c r="H30" s="183"/>
-      <c r="I30" s="206"/>
+      <c r="H30" s="186"/>
+      <c r="I30" s="209"/>
     </row>
     <row r="31" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="73"/>
@@ -4849,8 +4875,8 @@
       <c r="E31" s="79"/>
       <c r="F31" s="79"/>
       <c r="G31" s="138"/>
-      <c r="H31" s="183"/>
-      <c r="I31" s="206"/>
+      <c r="H31" s="186"/>
+      <c r="I31" s="209"/>
     </row>
     <row r="32" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="73"/>
@@ -4860,8 +4886,8 @@
       <c r="E32" s="79"/>
       <c r="F32" s="79"/>
       <c r="G32" s="138"/>
-      <c r="H32" s="183"/>
-      <c r="I32" s="206"/>
+      <c r="H32" s="186"/>
+      <c r="I32" s="209"/>
     </row>
     <row r="33" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="73"/>
@@ -4871,8 +4897,8 @@
       <c r="E33" s="79"/>
       <c r="F33" s="79"/>
       <c r="G33" s="138"/>
-      <c r="H33" s="183"/>
-      <c r="I33" s="206"/>
+      <c r="H33" s="186"/>
+      <c r="I33" s="209"/>
     </row>
     <row r="34" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="73"/>
@@ -4882,8 +4908,8 @@
       <c r="E34" s="79"/>
       <c r="F34" s="79"/>
       <c r="G34" s="138"/>
-      <c r="H34" s="183"/>
-      <c r="I34" s="206"/>
+      <c r="H34" s="186"/>
+      <c r="I34" s="209"/>
     </row>
     <row r="35" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="73"/>
@@ -4893,8 +4919,8 @@
       <c r="E35" s="79"/>
       <c r="F35" s="79"/>
       <c r="G35" s="138"/>
-      <c r="H35" s="183"/>
-      <c r="I35" s="206"/>
+      <c r="H35" s="186"/>
+      <c r="I35" s="209"/>
     </row>
     <row r="36" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="73"/>
@@ -4904,8 +4930,8 @@
       <c r="E36" s="79"/>
       <c r="F36" s="79"/>
       <c r="G36" s="138"/>
-      <c r="H36" s="183"/>
-      <c r="I36" s="206"/>
+      <c r="H36" s="186"/>
+      <c r="I36" s="209"/>
     </row>
     <row r="37" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="73"/>
@@ -4915,8 +4941,8 @@
       <c r="E37" s="79"/>
       <c r="F37" s="79"/>
       <c r="G37" s="138"/>
-      <c r="H37" s="183"/>
-      <c r="I37" s="206"/>
+      <c r="H37" s="186"/>
+      <c r="I37" s="209"/>
     </row>
     <row r="38" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="73"/>
@@ -4926,16 +4952,16 @@
       <c r="E38" s="93"/>
       <c r="F38" s="93"/>
       <c r="G38" s="140"/>
-      <c r="H38" s="183"/>
-      <c r="I38" s="206"/>
+      <c r="H38" s="186"/>
+      <c r="I38" s="209"/>
     </row>
     <row r="39" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="169" t="s">
+      <c r="A39" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="170"/>
-      <c r="C39" s="170"/>
-      <c r="D39" s="122" t="e">
+      <c r="B39" s="169"/>
+      <c r="C39" s="291"/>
+      <c r="D39" s="288" t="e">
         <f>AVERAGE(D9:D38)</f>
         <v>#DIV/0!</v>
       </c>
@@ -4951,16 +4977,16 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="183"/>
-      <c r="I39" s="206"/>
+      <c r="H39" s="186"/>
+      <c r="I39" s="209"/>
     </row>
     <row r="40" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="167" t="s">
+      <c r="A40" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="168"/>
-      <c r="C40" s="168"/>
-      <c r="D40" s="124">
+      <c r="B40" s="171"/>
+      <c r="C40" s="292"/>
+      <c r="D40" s="289">
         <f>MIN(D9:D38)</f>
         <v>0</v>
       </c>
@@ -4976,16 +5002,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H40" s="183"/>
-      <c r="I40" s="206"/>
+      <c r="H40" s="186"/>
+      <c r="I40" s="209"/>
     </row>
     <row r="41" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="165" t="s">
+      <c r="A41" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="166"/>
-      <c r="C41" s="166"/>
-      <c r="D41" s="126">
+      <c r="B41" s="173"/>
+      <c r="C41" s="293"/>
+      <c r="D41" s="290">
         <f>MAX(D9:D38)</f>
         <v>0</v>
       </c>
@@ -5001,18 +5027,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H41" s="186"/>
-      <c r="I41" s="207"/>
+      <c r="H41" s="189"/>
+      <c r="I41" s="210"/>
     </row>
     <row r="42" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="172">
+      <c r="B42" s="192">
         <f>Page1!B42</f>
         <v>0</v>
       </c>
-      <c r="C42" s="189"/>
+      <c r="C42" s="193"/>
       <c r="D42" s="128" t="s">
         <v>16</v>
       </c>
@@ -5031,11 +5057,11 @@
     </row>
     <row r="43" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="132"/>
-      <c r="B43" s="173">
+      <c r="B43" s="176">
         <f>Page1!B43</f>
         <v>0</v>
       </c>
-      <c r="C43" s="190"/>
+      <c r="C43" s="194"/>
       <c r="D43" s="128"/>
       <c r="E43" s="128"/>
       <c r="F43" s="129"/>
@@ -5047,11 +5073,11 @@
       <c r="I43" s="131"/>
     </row>
     <row r="44" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="178" t="s">
+      <c r="A44" s="181" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="178"/>
-      <c r="C44" s="178"/>
+      <c r="B44" s="181"/>
+      <c r="C44" s="181"/>
       <c r="D44" s="133"/>
       <c r="E44" s="134" t="s">
         <v>109</v>
@@ -5065,19 +5091,19 @@
       <c r="I44" s="133"/>
     </row>
     <row r="45" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="178" t="s">
+      <c r="A45" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="178"/>
-      <c r="C45" s="178"/>
+      <c r="B45" s="181"/>
+      <c r="C45" s="181"/>
       <c r="D45" s="133"/>
       <c r="E45" s="133"/>
       <c r="F45" s="133"/>
       <c r="G45" s="133"/>
-      <c r="H45" s="179" t="s">
+      <c r="H45" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="I45" s="179"/>
+      <c r="I45" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -5086,9 +5112,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A45:C45"/>
@@ -5101,6 +5124,9 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
   </mergeCells>
   <conditionalFormatting sqref="D9:D38">
     <cfRule type="cellIs" dxfId="3" priority="6" operator="notBetween">
@@ -5153,15 +5179,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="216" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="217"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="218"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -5175,37 +5201,37 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="219" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="219"/>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="220"/>
+      <c r="B3" s="220"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="221"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182" t="s">
+      <c r="A4" s="185" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="221"/>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
-      <c r="E4" s="221"/>
-      <c r="F4" s="221"/>
-      <c r="G4" s="206"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
+      <c r="D4" s="222"/>
+      <c r="E4" s="222"/>
+      <c r="F4" s="222"/>
+      <c r="G4" s="209"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="222" t="s">
+      <c r="A5" s="223" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="223"/>
-      <c r="C5" s="223"/>
-      <c r="D5" s="223"/>
-      <c r="E5" s="223"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="224"/>
+      <c r="B5" s="224"/>
+      <c r="C5" s="224"/>
+      <c r="D5" s="224"/>
+      <c r="E5" s="224"/>
+      <c r="F5" s="224"/>
+      <c r="G5" s="225"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -5217,15 +5243,15 @@
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="225">
+      <c r="D6" s="226">
         <f>Page1!G4</f>
         <v>0</v>
       </c>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227" t="s">
+      <c r="E6" s="227"/>
+      <c r="F6" s="228" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="228">
+      <c r="G6" s="229">
         <f>Page1!I4</f>
         <v>0</v>
       </c>
@@ -5238,13 +5264,13 @@
       <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="225">
+      <c r="D7" s="226">
         <f>Page1!E5</f>
         <v>0</v>
       </c>
-      <c r="E7" s="226"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="229"/>
+      <c r="E7" s="227"/>
+      <c r="F7" s="228"/>
+      <c r="G7" s="230"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -5257,15 +5283,15 @@
       <c r="C8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="227">
+      <c r="D8" s="228">
         <f>Page1!G5</f>
         <v>0</v>
       </c>
-      <c r="E8" s="227"/>
-      <c r="F8" s="240" t="s">
+      <c r="E8" s="228"/>
+      <c r="F8" s="241" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="228">
+      <c r="G8" s="229">
         <f>Page1!I5</f>
         <v>0</v>
       </c>
@@ -5278,15 +5304,15 @@
         <f>Page1!F44</f>
         <v>461343000</v>
       </c>
-      <c r="C9" s="240" t="s">
+      <c r="C9" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="245" t="s">
+      <c r="D9" s="246" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="246"/>
-      <c r="F9" s="241"/>
-      <c r="G9" s="243"/>
+      <c r="E9" s="247"/>
+      <c r="F9" s="242"/>
+      <c r="G9" s="244"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
@@ -5296,34 +5322,34 @@
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C10" s="242"/>
-      <c r="D10" s="247"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="242"/>
-      <c r="G10" s="244"/>
+      <c r="C10" s="243"/>
+      <c r="D10" s="248"/>
+      <c r="E10" s="249"/>
+      <c r="F10" s="243"/>
+      <c r="G10" s="245"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="230" t="s">
+      <c r="A11" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="232" t="s">
+      <c r="B11" s="233" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="234" t="s">
+      <c r="C11" s="235" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="235"/>
-      <c r="E11" s="236"/>
-      <c r="F11" s="232" t="s">
+      <c r="D11" s="236"/>
+      <c r="E11" s="237"/>
+      <c r="F11" s="233" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="237" t="s">
+      <c r="G11" s="238" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="231"/>
-      <c r="B12" s="233"/>
+      <c r="A12" s="232"/>
+      <c r="B12" s="234"/>
       <c r="C12" s="14" t="s">
         <v>59</v>
       </c>
@@ -5333,8 +5359,8 @@
       <c r="E12" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="233"/>
-      <c r="G12" s="238"/>
+      <c r="F12" s="234"/>
+      <c r="G12" s="239"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
@@ -5404,7 +5430,7 @@
         <f>Page1!I39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="239" t="s">
+      <c r="G15" s="240" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5428,7 +5454,7 @@
         <f>Page2!F41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="180"/>
+      <c r="G16" s="183"/>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
@@ -5450,7 +5476,7 @@
         <f>Page1!G39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="180"/>
+      <c r="G17" s="183"/>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
@@ -5472,7 +5498,7 @@
         <f>Page2!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="180"/>
+      <c r="G18" s="183"/>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
@@ -5494,7 +5520,7 @@
         <f>Page1!H39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="180"/>
+      <c r="G19" s="183"/>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
@@ -5516,7 +5542,7 @@
         <f>Page2!E41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="180"/>
+      <c r="G20" s="183"/>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
@@ -5538,7 +5564,7 @@
         <f>Page1!F39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="180"/>
+      <c r="G21" s="183"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
@@ -5612,26 +5638,26 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="254" t="s">
+      <c r="A25" s="255" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="255"/>
-      <c r="C25" s="255"/>
-      <c r="D25" s="255"/>
-      <c r="E25" s="255"/>
-      <c r="F25" s="255"/>
-      <c r="G25" s="256"/>
+      <c r="B25" s="256"/>
+      <c r="C25" s="256"/>
+      <c r="D25" s="256"/>
+      <c r="E25" s="256"/>
+      <c r="F25" s="256"/>
+      <c r="G25" s="257"/>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="257" t="s">
+      <c r="A26" s="258" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="258"/>
-      <c r="C26" s="259" t="s">
+      <c r="B26" s="259"/>
+      <c r="C26" s="260" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="260"/>
-      <c r="E26" s="261"/>
+      <c r="D26" s="261"/>
+      <c r="E26" s="262"/>
       <c r="F26" s="32" t="s">
         <v>86</v>
       </c>
@@ -5640,15 +5666,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="262" t="s">
+      <c r="A27" s="263" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="226"/>
-      <c r="C27" s="263" t="s">
+      <c r="B27" s="227"/>
+      <c r="C27" s="264" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="264"/>
-      <c r="E27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="266"/>
       <c r="F27" s="33" t="s">
         <v>86</v>
       </c>
@@ -5657,15 +5683,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="262" t="s">
+      <c r="A28" s="263" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="226"/>
-      <c r="C28" s="263" t="s">
+      <c r="B28" s="227"/>
+      <c r="C28" s="264" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="264"/>
-      <c r="E28" s="265"/>
+      <c r="D28" s="265"/>
+      <c r="E28" s="266"/>
       <c r="F28" s="33" t="s">
         <v>86</v>
       </c>
@@ -5674,15 +5700,15 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="262" t="s">
+      <c r="A29" s="263" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="226"/>
-      <c r="C29" s="263" t="s">
+      <c r="B29" s="227"/>
+      <c r="C29" s="264" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="264"/>
-      <c r="E29" s="265"/>
+      <c r="D29" s="265"/>
+      <c r="E29" s="266"/>
       <c r="F29" s="33" t="s">
         <v>86</v>
       </c>
@@ -5691,15 +5717,15 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="262" t="s">
+      <c r="A30" s="263" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="226"/>
-      <c r="C30" s="263" t="s">
+      <c r="B30" s="227"/>
+      <c r="C30" s="264" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="264"/>
-      <c r="E30" s="265"/>
+      <c r="D30" s="265"/>
+      <c r="E30" s="266"/>
       <c r="F30" s="33" t="s">
         <v>86</v>
       </c>
@@ -5708,15 +5734,15 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="249" t="s">
+      <c r="A31" s="250" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="250"/>
-      <c r="C31" s="251" t="s">
+      <c r="B31" s="251"/>
+      <c r="C31" s="252" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="252"/>
-      <c r="E31" s="253"/>
+      <c r="D31" s="253"/>
+      <c r="E31" s="254"/>
       <c r="F31" s="35" t="s">
         <v>86</v>
       </c>
@@ -5725,50 +5751,50 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="269" t="s">
+      <c r="A32" s="270" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="270"/>
-      <c r="C32" s="271" t="s">
+      <c r="B32" s="271"/>
+      <c r="C32" s="272" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="272"/>
-      <c r="E32" s="273"/>
-      <c r="F32" s="271" t="s">
+      <c r="D32" s="273"/>
+      <c r="E32" s="274"/>
+      <c r="F32" s="272" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="273"/>
+      <c r="G32" s="274"/>
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="274"/>
-      <c r="B33" s="275"/>
-      <c r="C33" s="278"/>
-      <c r="D33" s="279"/>
-      <c r="E33" s="280"/>
-      <c r="F33" s="278"/>
-      <c r="G33" s="280"/>
+      <c r="A33" s="275"/>
+      <c r="B33" s="276"/>
+      <c r="C33" s="279"/>
+      <c r="D33" s="280"/>
+      <c r="E33" s="281"/>
+      <c r="F33" s="279"/>
+      <c r="G33" s="281"/>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="276"/>
-      <c r="B34" s="277"/>
-      <c r="C34" s="281" t="s">
+      <c r="A34" s="277"/>
+      <c r="B34" s="278"/>
+      <c r="C34" s="282" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="282"/>
-      <c r="E34" s="283"/>
-      <c r="F34" s="281" t="s">
+      <c r="D34" s="283"/>
+      <c r="E34" s="284"/>
+      <c r="F34" s="282" t="s">
         <v>104</v>
       </c>
-      <c r="G34" s="283"/>
+      <c r="G34" s="284"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37"/>
       <c r="B35" s="37"/>
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
-      <c r="E35" s="266"/>
-      <c r="F35" s="266"/>
-      <c r="G35" s="266"/>
+      <c r="E35" s="267"/>
+      <c r="F35" s="267"/>
+      <c r="G35" s="267"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
@@ -5777,21 +5803,21 @@
       <c r="B36" s="39"/>
       <c r="C36" s="40"/>
       <c r="D36" s="37"/>
-      <c r="E36" s="267"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="267"/>
+      <c r="E36" s="268"/>
+      <c r="F36" s="268"/>
+      <c r="G36" s="268"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="268" t="s">
+      <c r="A38" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="268"/>
+      <c r="B38" s="269"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="268" t="s">
+      <c r="A39" s="269" t="s">
         <v>107</v>
       </c>
-      <c r="B39" s="268"/>
+      <c r="B39" s="269"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -5840,9 +5866,8 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="D7:E7"/>
   </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added digital signatures in FIF & added advanced fimter in PR
</commit_message>
<xml_diff>
--- a/backend/templates/UC-16gsm-165W.xlsx
+++ b/backend/templates/UC-16gsm-165W.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C581B3-519B-4173-A326-7974FD9E36AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6FAD99-7088-4754-B0E5-A92390B54540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
     <sheet name="COA Form" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'COA Form'!$A$1:$G$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'COA Form'!$A$1:$H$40</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Page1!$A$1:$I$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Page2!$A$1:$I$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Page3!$A$1:$I$45</definedName>
@@ -1348,7 +1348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1414,9 +1414,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1444,16 +1441,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2068,6 +2056,39 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2104,14 +2125,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2182,24 +2197,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2212,6 +2224,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2257,9 +2293,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2273,6 +2306,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2463,7 +2499,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>104118</xdr:rowOff>
@@ -2833,495 +2869,495 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="14" style="43" customWidth="1"/>
-    <col min="4" max="9" width="22.140625" style="43" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="43"/>
-    <col min="12" max="12" width="9.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="3" width="14" style="39" customWidth="1"/>
+    <col min="4" max="9" width="22.140625" style="39" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="39"/>
+    <col min="12" max="12" width="9.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+    <row r="1" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="54" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+    <row r="2" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="55" t="s">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+    <row r="3" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="52"/>
-    </row>
-    <row r="4" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="I3" s="48"/>
+    </row>
+    <row r="4" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="159"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="60" t="s">
+      <c r="B4" s="155"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="60" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="144" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="K4" s="42" t="s">
+      <c r="I4" s="57"/>
+      <c r="K4" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+    <row r="5" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="63" t="s">
+      <c r="B5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="147"/>
-      <c r="F5" s="63" t="s">
+      <c r="E5" s="143"/>
+      <c r="F5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="147"/>
+      <c r="G5" s="143"/>
       <c r="H5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="64"/>
-    </row>
-    <row r="6" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="172" t="s">
+      <c r="I5" s="60"/>
+    </row>
+    <row r="6" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="168" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="173"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="148"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="166"/>
-      <c r="H6" s="167"/>
-      <c r="I6" s="168"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="170"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="162"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="164"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="175" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="169"/>
-      <c r="C7" s="169"/>
-      <c r="D7" s="169" t="s">
+      <c r="A7" s="171" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="163" t="s">
+      <c r="E7" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="163" t="s">
+      <c r="F7" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="169" t="s">
+      <c r="G7" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="169"/>
-      <c r="I7" s="170"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="166"/>
     </row>
     <row r="8" spans="1:11" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="176"/>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="65" t="s">
+      <c r="A8" s="172"/>
+      <c r="B8" s="173"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="173"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="147" t="s">
+      <c r="H8" s="143" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="72"/>
-    </row>
-    <row r="10" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="80"/>
-    </row>
-    <row r="11" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="80"/>
-    </row>
-    <row r="12" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="80"/>
-    </row>
-    <row r="13" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="80"/>
-    </row>
-    <row r="14" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="80"/>
-    </row>
-    <row r="15" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="80"/>
-    </row>
-    <row r="16" spans="1:11" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="80"/>
-    </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="80"/>
-    </row>
-    <row r="18" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="80"/>
-    </row>
-    <row r="19" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="80"/>
-    </row>
-    <row r="20" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="80"/>
-    </row>
-    <row r="21" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="80"/>
-    </row>
-    <row r="22" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="86"/>
-    </row>
-    <row r="23" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="80"/>
-    </row>
-    <row r="24" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="80"/>
-    </row>
-    <row r="25" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="80"/>
-    </row>
-    <row r="26" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="80"/>
-    </row>
-    <row r="27" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="73"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="80"/>
-    </row>
-    <row r="28" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="80"/>
-    </row>
-    <row r="29" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="80"/>
-    </row>
-    <row r="30" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="80"/>
-    </row>
-    <row r="31" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="80"/>
-    </row>
-    <row r="32" spans="1:9" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="80"/>
-    </row>
-    <row r="33" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="80"/>
-    </row>
-    <row r="34" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="80"/>
-    </row>
-    <row r="35" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="80"/>
-    </row>
-    <row r="36" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="80"/>
-    </row>
-    <row r="37" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
-      <c r="B37" s="74"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="80"/>
-    </row>
-    <row r="38" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="88"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
-      <c r="H38" s="92"/>
-      <c r="I38" s="94"/>
-    </row>
-    <row r="39" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="178" t="s">
+    <row r="9" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="68"/>
+    </row>
+    <row r="10" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="69"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+    </row>
+    <row r="11" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="76"/>
+    </row>
+    <row r="12" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="76"/>
+    </row>
+    <row r="14" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="76"/>
+    </row>
+    <row r="15" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="69"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="76"/>
+    </row>
+    <row r="16" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="76"/>
+    </row>
+    <row r="17" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="76"/>
+    </row>
+    <row r="18" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="69"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="76"/>
+    </row>
+    <row r="19" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="69"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="76"/>
+    </row>
+    <row r="20" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="69"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="76"/>
+    </row>
+    <row r="21" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="76"/>
+    </row>
+    <row r="22" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="82"/>
+    </row>
+    <row r="23" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="76"/>
+    </row>
+    <row r="24" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="76"/>
+    </row>
+    <row r="25" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="69"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="76"/>
+    </row>
+    <row r="26" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="76"/>
+    </row>
+    <row r="27" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="76"/>
+    </row>
+    <row r="28" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="69"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="76"/>
+    </row>
+    <row r="29" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="69"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="76"/>
+    </row>
+    <row r="30" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="69"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="76"/>
+    </row>
+    <row r="31" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="69"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="76"/>
+    </row>
+    <row r="32" spans="1:9" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="76"/>
+    </row>
+    <row r="33" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="76"/>
+    </row>
+    <row r="34" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="70"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="76"/>
+    </row>
+    <row r="35" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="69"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="76"/>
+    </row>
+    <row r="36" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="76"/>
+    </row>
+    <row r="37" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="69"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="76"/>
+    </row>
+    <row r="38" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="84"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="90"/>
+    </row>
+    <row r="39" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="179"/>
-      <c r="C39" s="180"/>
-      <c r="D39" s="150" t="e">
+      <c r="B39" s="175"/>
+      <c r="C39" s="176"/>
+      <c r="D39" s="146" t="e">
         <f>AVERAGE(D9:D38)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E39" s="95" t="e">
+      <c r="E39" s="91" t="e">
         <f t="shared" ref="E39:H39" si="0">AVERAGE(E9:E38)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3333,152 +3369,152 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="95" t="e">
+      <c r="H39" s="91" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I39" s="123" t="e">
+      <c r="I39" s="119" t="e">
         <f t="shared" ref="I39" si="1">AVERAGE(I9:I38)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="181" t="s">
+    <row r="40" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="182"/>
-      <c r="C40" s="183"/>
-      <c r="D40" s="151">
+      <c r="B40" s="178"/>
+      <c r="C40" s="179"/>
+      <c r="D40" s="147">
         <f>MIN(D9:D38)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="23">
         <f t="shared" ref="E40:H40" si="2">MIN(E9:E38)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="25">
+      <c r="F40" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I40" s="125">
+      <c r="I40" s="121">
         <f t="shared" ref="I40" si="3">MIN(I9:I38)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="42" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="184" t="s">
+    <row r="41" spans="1:12" s="38" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="185"/>
-      <c r="C41" s="186"/>
-      <c r="D41" s="152">
+      <c r="B41" s="181"/>
+      <c r="C41" s="182"/>
+      <c r="D41" s="148">
         <f>MAX(D9:D38)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="97">
+      <c r="E41" s="93">
         <f t="shared" ref="E41:H41" si="4">MAX(E9:E38)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="96">
+      <c r="F41" s="92">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G41" s="96">
+      <c r="G41" s="92">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H41" s="97">
+      <c r="H41" s="93">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I41" s="127">
+      <c r="I41" s="123">
         <f t="shared" ref="I41" si="5">MAX(I9:I38)</f>
         <v>0</v>
       </c>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-    </row>
-    <row r="42" spans="1:12" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="98" t="s">
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+    </row>
+    <row r="42" spans="1:12" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="157"/>
-      <c r="C42" s="157"/>
-      <c r="D42" s="98" t="s">
+      <c r="B42" s="153"/>
+      <c r="C42" s="153"/>
+      <c r="D42" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="99"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="58" t="s">
+      <c r="E42" s="95"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="56"/>
-      <c r="I42" s="101" t="s">
+      <c r="H42" s="52"/>
+      <c r="I42" s="97" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="102"/>
-      <c r="B43" s="158"/>
-      <c r="C43" s="158"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="101"/>
+    <row r="43" spans="1:12" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="98"/>
+      <c r="B43" s="154"/>
+      <c r="C43" s="154"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="95"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="97"/>
     </row>
     <row r="44" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="171" t="s">
+      <c r="A44" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="171"/>
-      <c r="C44" s="171"/>
-      <c r="D44" s="103"/>
-      <c r="E44" s="104" t="s">
+      <c r="B44" s="167"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="53">
+      <c r="F44" s="49">
         <v>461343000</v>
       </c>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
     </row>
     <row r="45" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="171" t="s">
+      <c r="A45" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="171"/>
-      <c r="C45" s="171"/>
-      <c r="D45" s="103"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="165" t="s">
+      <c r="B45" s="167"/>
+      <c r="C45" s="167"/>
+      <c r="D45" s="99"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="I45" s="165"/>
+      <c r="I45" s="161"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -3550,842 +3586,842 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="13.85546875" style="50" customWidth="1"/>
-    <col min="4" max="9" width="22.140625" style="50" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="50"/>
+    <col min="1" max="3" width="13.85546875" style="46" customWidth="1"/>
+    <col min="4" max="9" width="22.140625" style="46" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+    <row r="1" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="54" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+    <row r="2" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="55" t="s">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+    <row r="3" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="48">
         <f>Page1!I3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="159">
+      <c r="B4" s="155">
         <f>Page1!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="60" t="s">
+      <c r="C4" s="156"/>
+      <c r="D4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="32">
         <f>Page1!E4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="32">
         <f>Page1!G4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="144" t="s">
+      <c r="H4" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="57">
         <f>Page1!I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105" t="s">
+    <row r="5" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="187">
+      <c r="B5" s="183">
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="106" t="s">
+      <c r="C5" s="184"/>
+      <c r="D5" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <f>Page1!E5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <f>Page1!G5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="149" t="s">
+      <c r="H5" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="107">
+      <c r="I5" s="103">
         <f>Page1!I5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="49" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="195" t="s">
+    <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="191" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="196"/>
-      <c r="C6" s="196"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="167"/>
-      <c r="F6" s="197"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="110"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="193"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="106"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="206"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="198" t="s">
+      <c r="A7" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="202"/>
+      <c r="C7" s="189"/>
+      <c r="D7" s="194" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="199"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="209" t="s">
+      <c r="E7" s="195"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="205" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="203" t="s">
+      <c r="I7" s="199" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="205"/>
-      <c r="B8" s="206"/>
-      <c r="C8" s="193"/>
-      <c r="D8" s="189" t="s">
+      <c r="A8" s="201"/>
+      <c r="B8" s="202"/>
+      <c r="C8" s="189"/>
+      <c r="D8" s="185" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="192" t="s">
+      <c r="E8" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="188" t="s">
+      <c r="F8" s="184" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="209"/>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="205"/>
+      <c r="H8" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="I8" s="203"/>
+      <c r="I8" s="199"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="205"/>
-      <c r="B9" s="206"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="190"/>
-      <c r="E9" s="192"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="209"/>
-      <c r="H9" s="46" t="s">
+      <c r="A9" s="201"/>
+      <c r="B9" s="202"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="188"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="I9" s="203"/>
+      <c r="I9" s="199"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="207"/>
-      <c r="B10" s="208"/>
-      <c r="C10" s="194"/>
-      <c r="D10" s="191"/>
-      <c r="E10" s="177"/>
-      <c r="F10" s="194"/>
-      <c r="G10" s="164"/>
-      <c r="H10" s="47" t="s">
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="187"/>
+      <c r="E10" s="173"/>
+      <c r="F10" s="190"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="204"/>
-    </row>
-    <row r="11" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="111"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="86"/>
-    </row>
-    <row r="12" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="80"/>
-    </row>
-    <row r="13" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="80"/>
-    </row>
-    <row r="14" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="80"/>
-    </row>
-    <row r="15" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="80"/>
-    </row>
-    <row r="16" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="80"/>
-    </row>
-    <row r="17" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="116"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="80"/>
-    </row>
-    <row r="18" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="116"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="80"/>
-    </row>
-    <row r="19" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="80"/>
-    </row>
-    <row r="20" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="117"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="80"/>
-    </row>
-    <row r="21" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="116"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="80"/>
-    </row>
-    <row r="22" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="80"/>
-    </row>
-    <row r="23" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="117"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="80"/>
-    </row>
-    <row r="24" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="117"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="80"/>
-    </row>
-    <row r="25" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="114"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="86"/>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="86"/>
-    </row>
-    <row r="27" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="73"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="86"/>
-    </row>
-    <row r="28" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="114"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="86"/>
-    </row>
-    <row r="29" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="113" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H29" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29" s="86" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="113" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="114" t="s">
-        <v>117</v>
-      </c>
-      <c r="G30" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I30" s="86" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G31" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I31" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="116"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E32" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F32" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H32" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="116"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F33" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G33" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H33" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H34" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I34" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F35" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G35" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H35" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G36" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H36" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F37" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H37" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I37" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="73"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G38" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H38" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I38" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="73"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="118" t="s">
-        <v>117</v>
-      </c>
-      <c r="H39" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="I39" s="80" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="73"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="119" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="F40" s="120" t="s">
-        <v>117</v>
-      </c>
-      <c r="G40" s="121" t="s">
-        <v>117</v>
-      </c>
-      <c r="H40" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" s="94" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="178" t="s">
+      <c r="I10" s="200"/>
+    </row>
+    <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="107"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="82"/>
+    </row>
+    <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="69"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="76"/>
+    </row>
+    <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="69"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="114"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="76"/>
+    </row>
+    <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="69"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="76"/>
+    </row>
+    <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="76"/>
+    </row>
+    <row r="17" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="76"/>
+    </row>
+    <row r="18" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="69"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="76"/>
+    </row>
+    <row r="19" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="69"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="113"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="76"/>
+    </row>
+    <row r="20" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="69"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="114"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="76"/>
+    </row>
+    <row r="21" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="114"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="76"/>
+    </row>
+    <row r="22" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="69"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="114"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="76"/>
+    </row>
+    <row r="23" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="76"/>
+    </row>
+    <row r="24" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="76"/>
+    </row>
+    <row r="25" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="69"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="114"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="82"/>
+    </row>
+    <row r="26" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="82"/>
+    </row>
+    <row r="27" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="69"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="82"/>
+    </row>
+    <row r="28" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="69"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="114"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="82"/>
+    </row>
+    <row r="29" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="69"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" s="82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="69"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="110" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I30" s="82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="69"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="69"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="69"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H35" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H36" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I36" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="69"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="69"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I38" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="69"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="113" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="H39" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="I39" s="76" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="69"/>
+      <c r="B40" s="112"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="115" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="116" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="117" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" s="90" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="179"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="150" t="e">
+      <c r="B41" s="175"/>
+      <c r="C41" s="176"/>
+      <c r="D41" s="146" t="e">
         <f>AVERAGE(D11:D40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E41" s="95" t="e">
+      <c r="E41" s="91" t="e">
         <f t="shared" ref="E41:I41" si="0">AVERAGE(E11:E40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F41" s="95" t="e">
+      <c r="F41" s="91" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G41" s="122" t="e">
+      <c r="G41" s="118" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H41" s="95" t="e">
+      <c r="H41" s="91" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I41" s="123" t="e">
+      <c r="I41" s="119" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="181" t="s">
+    <row r="42" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="182"/>
-      <c r="C42" s="183"/>
-      <c r="D42" s="151">
+      <c r="B42" s="178"/>
+      <c r="C42" s="179"/>
+      <c r="D42" s="147">
         <f>MIN(D11:D40)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="23">
         <f t="shared" ref="E42:I42" si="1">MIN(E11:E40)</f>
         <v>0</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G42" s="124">
+      <c r="G42" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I42" s="125">
+      <c r="I42" s="121">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="184" t="s">
+      <c r="A43" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="185"/>
-      <c r="C43" s="186"/>
-      <c r="D43" s="152">
+      <c r="B43" s="181"/>
+      <c r="C43" s="182"/>
+      <c r="D43" s="148">
         <f>MAX(D11:D40)</f>
         <v>0</v>
       </c>
-      <c r="E43" s="97">
+      <c r="E43" s="93">
         <f t="shared" ref="E43:I43" si="2">MAX(E11:E40)</f>
         <v>0</v>
       </c>
-      <c r="F43" s="97">
+      <c r="F43" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G43" s="126">
+      <c r="G43" s="122">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H43" s="97">
+      <c r="H43" s="93">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I43" s="127">
+      <c r="I43" s="123">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="128" t="s">
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="210">
+      <c r="B44" s="206">
         <f>Page1!B42</f>
         <v>0</v>
       </c>
-      <c r="C44" s="211"/>
-      <c r="D44" s="128" t="s">
+      <c r="C44" s="207"/>
+      <c r="D44" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="128"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="129" t="s">
+      <c r="E44" s="124"/>
+      <c r="F44" s="125"/>
+      <c r="G44" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="130">
+      <c r="H44" s="126">
         <f>Page1!H42</f>
         <v>0</v>
       </c>
-      <c r="I44" s="131" t="s">
+      <c r="I44" s="127" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="132"/>
-      <c r="B45" s="158">
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="128"/>
+      <c r="B45" s="154">
         <f>Page1!B43</f>
         <v>0</v>
       </c>
-      <c r="C45" s="212"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="129"/>
-      <c r="G45" s="132"/>
-      <c r="H45" s="130">
+      <c r="C45" s="208"/>
+      <c r="D45" s="124"/>
+      <c r="E45" s="124"/>
+      <c r="F45" s="125"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="126">
         <f>Page1!H43</f>
         <v>0</v>
       </c>
-      <c r="I45" s="131"/>
-    </row>
-    <row r="46" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="201" t="s">
+      <c r="I45" s="127"/>
+    </row>
+    <row r="46" spans="1:9" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="197" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="201"/>
-      <c r="C46" s="201"/>
-      <c r="D46" s="133"/>
-      <c r="E46" s="134" t="s">
+      <c r="B46" s="197"/>
+      <c r="C46" s="197"/>
+      <c r="D46" s="129"/>
+      <c r="E46" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="132">
+      <c r="F46" s="128">
         <f>Page1!F44</f>
         <v>461343000</v>
       </c>
-      <c r="G46" s="133"/>
-      <c r="H46" s="133"/>
-      <c r="I46" s="133"/>
-    </row>
-    <row r="47" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="201" t="s">
+      <c r="G46" s="129"/>
+      <c r="H46" s="129"/>
+      <c r="I46" s="129"/>
+    </row>
+    <row r="47" spans="1:9" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="197" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="201"/>
-      <c r="C47" s="201"/>
-      <c r="D47" s="133"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="133"/>
-      <c r="G47" s="133"/>
-      <c r="H47" s="202" t="s">
+      <c r="B47" s="197"/>
+      <c r="C47" s="197"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="129"/>
+      <c r="F47" s="129"/>
+      <c r="G47" s="129"/>
+      <c r="H47" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="I47" s="202"/>
+      <c r="I47" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -4464,646 +4500,646 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="14" style="50" customWidth="1"/>
-    <col min="4" max="9" width="22.140625" style="50" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="50"/>
+    <col min="1" max="3" width="14" style="46" customWidth="1"/>
+    <col min="4" max="9" width="22.140625" style="46" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+    <row r="1" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="152" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156"/>
-      <c r="I1" s="54" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="156" t="s">
+    <row r="2" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="55" t="s">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="42" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58" t="s">
+    <row r="3" spans="1:11" s="38" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="48">
         <f>Page1!I3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="159">
+      <c r="B4" s="155">
         <f>Page1!B4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="60" t="s">
+      <c r="C4" s="156"/>
+      <c r="D4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="32">
         <f>Page1!E4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="32">
         <f>Page1!G4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="144" t="s">
+      <c r="H4" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="61">
+      <c r="I4" s="57">
         <f>Page1!I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="42" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105" t="s">
+    <row r="5" spans="1:11" s="38" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="187">
+      <c r="B5" s="183">
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="188"/>
-      <c r="D5" s="106" t="s">
+      <c r="C5" s="184"/>
+      <c r="D5" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <f>Page1!E5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="106" t="s">
+      <c r="F5" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <f>Page1!G5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="149" t="s">
+      <c r="H5" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="107">
+      <c r="I5" s="103">
         <f>Page1!I5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="49" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="195" t="s">
+    <row r="6" spans="1:11" s="45" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="191" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="196"/>
-      <c r="C6" s="196"/>
-      <c r="D6" s="167"/>
-      <c r="E6" s="167"/>
-      <c r="F6" s="167"/>
-      <c r="G6" s="168"/>
-      <c r="H6" s="213"/>
-      <c r="I6" s="214"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="209"/>
+      <c r="I6" s="210"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="217" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="213"/>
-      <c r="C7" s="218"/>
-      <c r="D7" s="219" t="s">
+      <c r="A7" s="213" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="209"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="215" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="221" t="s">
+      <c r="E7" s="217" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="221" t="s">
+      <c r="F7" s="217" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="223" t="s">
+      <c r="G7" s="219" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="206"/>
-      <c r="I7" s="215"/>
+      <c r="H7" s="202"/>
+      <c r="I7" s="211"/>
     </row>
     <row r="8" spans="1:11" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="207"/>
-      <c r="B8" s="208"/>
-      <c r="C8" s="194"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="222"/>
-      <c r="F8" s="222"/>
-      <c r="G8" s="224"/>
-      <c r="H8" s="206"/>
-      <c r="I8" s="215"/>
-    </row>
-    <row r="9" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="135"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="206"/>
-      <c r="I9" s="215"/>
-    </row>
-    <row r="10" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="137"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="138"/>
-      <c r="H10" s="206"/>
-      <c r="I10" s="215"/>
-    </row>
-    <row r="11" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
-      <c r="B11" s="116"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="206"/>
-      <c r="I11" s="215"/>
-    </row>
-    <row r="12" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="73"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="137"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="138"/>
-      <c r="H12" s="206"/>
-      <c r="I12" s="215"/>
-    </row>
-    <row r="13" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="73"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="137"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="206"/>
-      <c r="I13" s="215"/>
-    </row>
-    <row r="14" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="206"/>
-      <c r="I14" s="215"/>
-    </row>
-    <row r="15" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="206"/>
-      <c r="I15" s="215"/>
-    </row>
-    <row r="16" spans="1:11" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="137"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="206"/>
-      <c r="I16" s="215"/>
-    </row>
-    <row r="17" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="73"/>
-      <c r="B17" s="116"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="206"/>
-      <c r="I17" s="215"/>
-    </row>
-    <row r="18" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="116"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="206"/>
-      <c r="I18" s="215"/>
-    </row>
-    <row r="19" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="206"/>
-      <c r="I19" s="215"/>
-    </row>
-    <row r="20" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="206"/>
-      <c r="I20" s="215"/>
-    </row>
-    <row r="21" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="116"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="215"/>
-    </row>
-    <row r="22" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="206"/>
-      <c r="I22" s="215"/>
-    </row>
-    <row r="23" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="206"/>
-      <c r="I23" s="215"/>
-    </row>
-    <row r="24" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="135"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="136"/>
-      <c r="H24" s="206"/>
-      <c r="I24" s="215"/>
-    </row>
-    <row r="25" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="206"/>
-      <c r="I25" s="215"/>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="137"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="206"/>
-      <c r="I26" s="215"/>
-    </row>
-    <row r="27" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="73"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="206"/>
-      <c r="I27" s="215"/>
-    </row>
-    <row r="28" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="73"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="137"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="206"/>
-      <c r="I28" s="215"/>
-    </row>
-    <row r="29" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="137"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="206"/>
-      <c r="I29" s="215"/>
-    </row>
-    <row r="30" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="73"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="137"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="206"/>
-      <c r="I30" s="215"/>
-    </row>
-    <row r="31" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="137"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="215"/>
-    </row>
-    <row r="32" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="73"/>
-      <c r="B32" s="116"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="137"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="206"/>
-      <c r="I32" s="215"/>
-    </row>
-    <row r="33" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="116"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="137"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="138"/>
-      <c r="H33" s="206"/>
-      <c r="I33" s="215"/>
-    </row>
-    <row r="34" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="137"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="206"/>
-      <c r="I34" s="215"/>
-    </row>
-    <row r="35" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="137"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="206"/>
-      <c r="I35" s="215"/>
-    </row>
-    <row r="36" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="137"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="138"/>
-      <c r="H36" s="206"/>
-      <c r="I36" s="215"/>
-    </row>
-    <row r="37" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="138"/>
-      <c r="H37" s="206"/>
-      <c r="I37" s="215"/>
-    </row>
-    <row r="38" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="73"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="139"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="93"/>
-      <c r="G38" s="140"/>
-      <c r="H38" s="206"/>
-      <c r="I38" s="215"/>
-    </row>
-    <row r="39" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="178" t="s">
+      <c r="A8" s="203"/>
+      <c r="B8" s="204"/>
+      <c r="C8" s="190"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="218"/>
+      <c r="F8" s="218"/>
+      <c r="G8" s="220"/>
+      <c r="H8" s="202"/>
+      <c r="I8" s="211"/>
+    </row>
+    <row r="9" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="211"/>
+    </row>
+    <row r="10" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="69"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="134"/>
+      <c r="H10" s="202"/>
+      <c r="I10" s="211"/>
+    </row>
+    <row r="11" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="69"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="202"/>
+      <c r="I11" s="211"/>
+    </row>
+    <row r="12" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="202"/>
+      <c r="I12" s="211"/>
+    </row>
+    <row r="13" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="69"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="202"/>
+      <c r="I13" s="211"/>
+    </row>
+    <row r="14" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="69"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="211"/>
+    </row>
+    <row r="15" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="69"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="133"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="211"/>
+    </row>
+    <row r="16" spans="1:11" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="69"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="202"/>
+      <c r="I16" s="211"/>
+    </row>
+    <row r="17" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="134"/>
+      <c r="H17" s="202"/>
+      <c r="I17" s="211"/>
+    </row>
+    <row r="18" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="69"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="134"/>
+      <c r="H18" s="202"/>
+      <c r="I18" s="211"/>
+    </row>
+    <row r="19" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="69"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="134"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="211"/>
+    </row>
+    <row r="20" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="69"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="134"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="211"/>
+    </row>
+    <row r="21" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="134"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="211"/>
+    </row>
+    <row r="22" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="69"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="211"/>
+    </row>
+    <row r="23" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="211"/>
+    </row>
+    <row r="24" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="132"/>
+      <c r="H24" s="202"/>
+      <c r="I24" s="211"/>
+    </row>
+    <row r="25" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="69"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="202"/>
+      <c r="I25" s="211"/>
+    </row>
+    <row r="26" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="202"/>
+      <c r="I26" s="211"/>
+    </row>
+    <row r="27" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="69"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="202"/>
+      <c r="I27" s="211"/>
+    </row>
+    <row r="28" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="69"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="202"/>
+      <c r="I28" s="211"/>
+    </row>
+    <row r="29" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="69"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="202"/>
+      <c r="I29" s="211"/>
+    </row>
+    <row r="30" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="69"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="202"/>
+      <c r="I30" s="211"/>
+    </row>
+    <row r="31" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="69"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="202"/>
+      <c r="I31" s="211"/>
+    </row>
+    <row r="32" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="202"/>
+      <c r="I32" s="211"/>
+    </row>
+    <row r="33" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="69"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="202"/>
+      <c r="I33" s="211"/>
+    </row>
+    <row r="34" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="133"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="202"/>
+      <c r="I34" s="211"/>
+    </row>
+    <row r="35" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="69"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="134"/>
+      <c r="H35" s="202"/>
+      <c r="I35" s="211"/>
+    </row>
+    <row r="36" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="133"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="134"/>
+      <c r="H36" s="202"/>
+      <c r="I36" s="211"/>
+    </row>
+    <row r="37" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="69"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="133"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="134"/>
+      <c r="H37" s="202"/>
+      <c r="I37" s="211"/>
+    </row>
+    <row r="38" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="69"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="135"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="136"/>
+      <c r="H38" s="202"/>
+      <c r="I38" s="211"/>
+    </row>
+    <row r="39" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="179"/>
-      <c r="C39" s="180"/>
-      <c r="D39" s="153" t="e">
+      <c r="B39" s="175"/>
+      <c r="C39" s="176"/>
+      <c r="D39" s="149" t="e">
         <f>AVERAGE(D9:D38)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E39" s="122" t="e">
+      <c r="E39" s="118" t="e">
         <f t="shared" ref="E39:G39" si="0">AVERAGE(E9:E38)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F39" s="122" t="e">
+      <c r="F39" s="118" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G39" s="141" t="e">
+      <c r="G39" s="137" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H39" s="206"/>
-      <c r="I39" s="215"/>
-    </row>
-    <row r="40" spans="1:9" s="49" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="181" t="s">
+      <c r="H39" s="202"/>
+      <c r="I39" s="211"/>
+    </row>
+    <row r="40" spans="1:9" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="182"/>
-      <c r="C40" s="183"/>
-      <c r="D40" s="154">
+      <c r="B40" s="178"/>
+      <c r="C40" s="179"/>
+      <c r="D40" s="150">
         <f>MIN(D9:D38)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="124">
+      <c r="E40" s="120">
         <f t="shared" ref="E40:G40" si="1">MIN(E9:E38)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="124">
+      <c r="F40" s="120">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G40" s="142">
+      <c r="G40" s="138">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H40" s="206"/>
-      <c r="I40" s="215"/>
+      <c r="H40" s="202"/>
+      <c r="I40" s="211"/>
     </row>
     <row r="41" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="184" t="s">
+      <c r="A41" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="185"/>
-      <c r="C41" s="186"/>
-      <c r="D41" s="155">
+      <c r="B41" s="181"/>
+      <c r="C41" s="182"/>
+      <c r="D41" s="151">
         <f>MAX(D9:D38)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="126">
+      <c r="E41" s="122">
         <f t="shared" ref="E41:G41" si="2">MAX(E9:E38)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="126">
+      <c r="F41" s="122">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G41" s="143">
+      <c r="G41" s="139">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H41" s="208"/>
-      <c r="I41" s="216"/>
-    </row>
-    <row r="42" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="128" t="s">
+      <c r="H41" s="204"/>
+      <c r="I41" s="212"/>
+    </row>
+    <row r="42" spans="1:9" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="210">
+      <c r="B42" s="206">
         <f>Page1!B42</f>
         <v>0</v>
       </c>
-      <c r="C42" s="211"/>
-      <c r="D42" s="128" t="s">
+      <c r="C42" s="207"/>
+      <c r="D42" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="128"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="129" t="s">
+      <c r="E42" s="124"/>
+      <c r="F42" s="125"/>
+      <c r="G42" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="130">
+      <c r="H42" s="126">
         <f>Page1!H42</f>
         <v>0</v>
       </c>
-      <c r="I42" s="131" t="s">
+      <c r="I42" s="127" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="42" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="132"/>
-      <c r="B43" s="158">
+    <row r="43" spans="1:9" s="38" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="128"/>
+      <c r="B43" s="154">
         <f>Page1!B43</f>
         <v>0</v>
       </c>
-      <c r="C43" s="212"/>
-      <c r="D43" s="128"/>
-      <c r="E43" s="128"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="132"/>
-      <c r="H43" s="130">
+      <c r="C43" s="208"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="125"/>
+      <c r="G43" s="128"/>
+      <c r="H43" s="126">
         <f>Page1!H43</f>
         <v>0</v>
       </c>
-      <c r="I43" s="131"/>
-    </row>
-    <row r="44" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="201" t="s">
+      <c r="I43" s="127"/>
+    </row>
+    <row r="44" spans="1:9" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="197" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="201"/>
-      <c r="C44" s="201"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="134" t="s">
+      <c r="B44" s="197"/>
+      <c r="C44" s="197"/>
+      <c r="D44" s="129"/>
+      <c r="E44" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="132">
+      <c r="F44" s="128">
         <f>Page1!F44</f>
         <v>461343000</v>
       </c>
-      <c r="G44" s="133"/>
-      <c r="H44" s="133"/>
-      <c r="I44" s="133"/>
-    </row>
-    <row r="45" spans="1:9" s="43" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="201" t="s">
+      <c r="G44" s="129"/>
+      <c r="H44" s="129"/>
+      <c r="I44" s="129"/>
+    </row>
+    <row r="45" spans="1:9" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="197" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="201"/>
-      <c r="C45" s="201"/>
-      <c r="D45" s="133"/>
-      <c r="E45" s="133"/>
-      <c r="F45" s="133"/>
-      <c r="G45" s="133"/>
-      <c r="H45" s="202" t="s">
+      <c r="B45" s="197"/>
+      <c r="C45" s="197"/>
+      <c r="D45" s="129"/>
+      <c r="E45" s="129"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="129"/>
+      <c r="H45" s="198" t="s">
         <v>28</v>
       </c>
-      <c r="I45" s="202"/>
+      <c r="I45" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -5163,77 +5199,83 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="21.42578125" style="1" customWidth="1"/>
     <col min="3" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="38"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="282" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="294" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="283"/>
-      <c r="C1" s="283"/>
-      <c r="D1" s="283"/>
-      <c r="E1" s="283"/>
-      <c r="F1" s="283"/>
-      <c r="G1" s="284"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="295"/>
+      <c r="C1" s="295"/>
+      <c r="D1" s="295"/>
+      <c r="E1" s="295"/>
+      <c r="F1" s="295"/>
+      <c r="G1" s="295"/>
+      <c r="H1" s="296"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="285" t="s">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="297" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="286"/>
-      <c r="C3" s="286"/>
-      <c r="D3" s="286"/>
-      <c r="E3" s="286"/>
-      <c r="F3" s="286"/>
-      <c r="G3" s="287"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="205" t="s">
+      <c r="B3" s="298"/>
+      <c r="C3" s="298"/>
+      <c r="D3" s="298"/>
+      <c r="E3" s="298"/>
+      <c r="F3" s="298"/>
+      <c r="G3" s="298"/>
+      <c r="H3" s="299"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="215"/>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="289" t="s">
+      <c r="B4" s="244"/>
+      <c r="C4" s="244"/>
+      <c r="D4" s="244"/>
+      <c r="E4" s="244"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="244"/>
+      <c r="H4" s="211"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="300" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="290"/>
-      <c r="C5" s="290"/>
-      <c r="D5" s="290"/>
-      <c r="E5" s="290"/>
-      <c r="F5" s="290"/>
-      <c r="G5" s="291"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="301"/>
+      <c r="C5" s="301"/>
+      <c r="D5" s="301"/>
+      <c r="E5" s="301"/>
+      <c r="F5" s="301"/>
+      <c r="G5" s="301"/>
+      <c r="H5" s="302"/>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
@@ -5243,20 +5285,21 @@
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="292">
+      <c r="D6" s="303">
         <f>Page1!G4</f>
         <v>0</v>
       </c>
-      <c r="E6" s="257"/>
-      <c r="F6" s="262" t="s">
+      <c r="E6" s="262"/>
+      <c r="F6" s="273" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="266">
+      <c r="G6" s="274"/>
+      <c r="H6" s="268">
         <f>Page1!I4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -5264,15 +5307,16 @@
       <c r="C7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="292">
+      <c r="D7" s="303">
         <f>Page1!E5</f>
         <v>0</v>
       </c>
-      <c r="E7" s="257"/>
-      <c r="F7" s="262"/>
-      <c r="G7" s="293"/>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="262"/>
+      <c r="F7" s="305"/>
+      <c r="G7" s="257"/>
+      <c r="H7" s="304"/>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -5283,20 +5327,21 @@
       <c r="C8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="262">
+      <c r="D8" s="267">
         <f>Page1!G5</f>
         <v>0</v>
       </c>
-      <c r="E8" s="262"/>
-      <c r="F8" s="263" t="s">
+      <c r="E8" s="267"/>
+      <c r="F8" s="273" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="266">
+      <c r="G8" s="274"/>
+      <c r="H8" s="268">
         <f>Page1!I5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>51</v>
       </c>
@@ -5304,17 +5349,18 @@
         <f>Page1!F44</f>
         <v>461343000</v>
       </c>
-      <c r="C9" s="263" t="s">
+      <c r="C9" s="271" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="269" t="s">
+      <c r="D9" s="273" t="s">
         <v>122</v>
       </c>
-      <c r="E9" s="270"/>
-      <c r="F9" s="264"/>
-      <c r="G9" s="267"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="274"/>
+      <c r="F9" s="277"/>
+      <c r="G9" s="278"/>
+      <c r="H9" s="269"/>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>53</v>
       </c>
@@ -5322,34 +5368,36 @@
         <f>Page1!B5</f>
         <v>0</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="271"/>
-      <c r="E10" s="272"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="268"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="273" t="s">
+      <c r="C10" s="272"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="276"/>
+      <c r="F10" s="275"/>
+      <c r="G10" s="276"/>
+      <c r="H10" s="270"/>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="285" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="275" t="s">
+      <c r="B11" s="287" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="277" t="s">
+      <c r="C11" s="289" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="278"/>
-      <c r="E11" s="279"/>
-      <c r="F11" s="275" t="s">
+      <c r="D11" s="290"/>
+      <c r="E11" s="291"/>
+      <c r="F11" s="279" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="280" t="s">
+      <c r="G11" s="280"/>
+      <c r="H11" s="292" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="274"/>
-      <c r="B12" s="276"/>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="286"/>
+      <c r="B12" s="288"/>
       <c r="C12" s="14" t="s">
         <v>58</v>
       </c>
@@ -5359,10 +5407,11 @@
       <c r="E12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="276"/>
-      <c r="G12" s="281"/>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="281"/>
+      <c r="G12" s="282"/>
+      <c r="H12" s="293"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>61</v>
       </c>
@@ -5378,15 +5427,16 @@
       <c r="E13" s="17">
         <v>18</v>
       </c>
-      <c r="F13" s="18" t="e">
+      <c r="F13" s="283" t="e">
         <f>Page1!D39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="284"/>
+      <c r="H13" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>64</v>
       </c>
@@ -5402,15 +5452,16 @@
       <c r="E14" s="21">
         <v>52</v>
       </c>
-      <c r="F14" s="22" t="e">
+      <c r="F14" s="226" t="e">
         <f>Page1!E39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="227"/>
+      <c r="H14" s="22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>67</v>
       </c>
@@ -5426,15 +5477,16 @@
       <c r="E15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="24" t="e">
+      <c r="F15" s="224" t="e">
         <f>Page1!I39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="261" t="s">
+      <c r="G15" s="225"/>
+      <c r="H15" s="266" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>71</v>
       </c>
@@ -5450,57 +5502,60 @@
       <c r="E16" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="24" t="e">
+      <c r="F16" s="224" t="e">
         <f>Page2!F41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G16" s="203"/>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="225"/>
+      <c r="H16" s="199"/>
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="24">
         <v>5</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <v>11</v>
       </c>
-      <c r="F17" s="25" t="e">
+      <c r="F17" s="224" t="e">
         <f>Page1!G39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G17" s="203"/>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="225"/>
+      <c r="H17" s="199"/>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="24">
         <v>3</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="24">
         <v>9</v>
       </c>
-      <c r="F18" s="25" t="e">
+      <c r="F18" s="224" t="e">
         <f>Page2!D41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G18" s="203"/>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="225"/>
+      <c r="H18" s="199"/>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>119</v>
       </c>
@@ -5516,13 +5571,14 @@
       <c r="E19" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="24" t="e">
+      <c r="F19" s="224" t="e">
         <f>Page1!H39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G19" s="203"/>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="225"/>
+      <c r="H19" s="199"/>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>120</v>
       </c>
@@ -5538,35 +5594,37 @@
       <c r="E20" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="24" t="e">
+      <c r="F20" s="224" t="e">
         <f>Page2!E41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G20" s="203"/>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="225"/>
+      <c r="H20" s="199"/>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="24">
         <v>0.3</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="24">
         <v>0.45</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="24">
         <v>0.6</v>
       </c>
-      <c r="F21" s="25" t="e">
+      <c r="F21" s="224" t="e">
         <f>Page1!F39</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G21" s="203"/>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="225"/>
+      <c r="H21" s="199"/>
+    </row>
+    <row r="22" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>76</v>
       </c>
@@ -5576,28 +5634,29 @@
       <c r="C22" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>165</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="23">
         <v>168</v>
       </c>
-      <c r="F22" s="24" t="e">
+      <c r="F22" s="226" t="e">
         <f>Page2!H41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="227"/>
+      <c r="H22" s="22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <v>6000</v>
       </c>
       <c r="D23" s="21" t="s">
@@ -5606,243 +5665,275 @@
       <c r="E23" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="226">
         <v>6000</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="227"/>
+      <c r="H23" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="28">
         <v>430</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>460</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="29">
         <v>510</v>
       </c>
-      <c r="F24" s="30" t="e">
+      <c r="F24" s="228" t="e">
         <f>Page2!I41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="229"/>
+      <c r="H24" s="30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="248" t="s">
+    <row r="25" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="253" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="249"/>
-      <c r="C25" s="249"/>
-      <c r="D25" s="249"/>
-      <c r="E25" s="249"/>
-      <c r="F25" s="249"/>
-      <c r="G25" s="250"/>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="251" t="s">
+      <c r="B25" s="254"/>
+      <c r="C25" s="254"/>
+      <c r="D25" s="254"/>
+      <c r="E25" s="254"/>
+      <c r="F25" s="254"/>
+      <c r="G25" s="254"/>
+      <c r="H25" s="255"/>
+    </row>
+    <row r="26" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="256" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="252"/>
-      <c r="C26" s="253" t="s">
+      <c r="B26" s="257"/>
+      <c r="C26" s="258" t="s">
         <v>121</v>
       </c>
-      <c r="D26" s="254"/>
-      <c r="E26" s="255"/>
-      <c r="F26" s="32" t="s">
+      <c r="D26" s="259"/>
+      <c r="E26" s="260"/>
+      <c r="F26" s="230" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="231"/>
+      <c r="H26" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="256" t="s">
+    <row r="27" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="261" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="257"/>
-      <c r="C27" s="258" t="s">
+      <c r="B27" s="262"/>
+      <c r="C27" s="263" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="259"/>
-      <c r="E27" s="260"/>
-      <c r="F27" s="33" t="s">
+      <c r="D27" s="264"/>
+      <c r="E27" s="265"/>
+      <c r="F27" s="221" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="221"/>
+      <c r="H27" s="22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="256" t="s">
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="261" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="257"/>
-      <c r="C28" s="258" t="s">
+      <c r="B28" s="262"/>
+      <c r="C28" s="263" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="259"/>
-      <c r="E28" s="260"/>
-      <c r="F28" s="33" t="s">
+      <c r="D28" s="264"/>
+      <c r="E28" s="265"/>
+      <c r="F28" s="221" t="s">
         <v>85</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="221"/>
+      <c r="H28" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="256" t="s">
+    <row r="29" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="261" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="257"/>
-      <c r="C29" s="258" t="s">
+      <c r="B29" s="262"/>
+      <c r="C29" s="263" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="259"/>
-      <c r="E29" s="260"/>
-      <c r="F29" s="33" t="s">
+      <c r="D29" s="264"/>
+      <c r="E29" s="265"/>
+      <c r="F29" s="221" t="s">
         <v>85</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="G29" s="221"/>
+      <c r="H29" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="256" t="s">
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="261" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="257"/>
-      <c r="C30" s="258" t="s">
+      <c r="B30" s="262"/>
+      <c r="C30" s="263" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="259"/>
-      <c r="E30" s="260"/>
-      <c r="F30" s="33" t="s">
+      <c r="D30" s="264"/>
+      <c r="E30" s="265"/>
+      <c r="F30" s="221" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="221"/>
+      <c r="H30" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="243" t="s">
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="248" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="244"/>
-      <c r="C31" s="245" t="s">
+      <c r="B31" s="249"/>
+      <c r="C31" s="250" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="246"/>
-      <c r="E31" s="247"/>
-      <c r="F31" s="35" t="s">
+      <c r="D31" s="251"/>
+      <c r="E31" s="252"/>
+      <c r="F31" s="222" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="51" t="s">
+      <c r="G31" s="223"/>
+      <c r="H31" s="47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="228" t="s">
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="235" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="229"/>
-      <c r="C32" s="230" t="s">
+      <c r="B32" s="236"/>
+      <c r="C32" s="237" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="231"/>
-      <c r="E32" s="232"/>
-      <c r="F32" s="230" t="s">
+      <c r="D32" s="238"/>
+      <c r="E32" s="239"/>
+      <c r="F32" s="237" t="s">
         <v>102</v>
       </c>
-      <c r="G32" s="232"/>
-    </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="233"/>
-      <c r="B33" s="234"/>
-      <c r="C33" s="237"/>
-      <c r="D33" s="238"/>
-      <c r="E33" s="239"/>
-      <c r="F33" s="237"/>
-      <c r="G33" s="239"/>
-    </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="235"/>
-      <c r="B34" s="236"/>
-      <c r="C34" s="240" t="s">
+      <c r="G32" s="238"/>
+      <c r="H32" s="239"/>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="240"/>
+      <c r="B33" s="241"/>
+      <c r="C33" s="201"/>
+      <c r="D33" s="244"/>
+      <c r="E33" s="211"/>
+      <c r="F33" s="201"/>
+      <c r="G33" s="202"/>
+      <c r="H33" s="211"/>
+    </row>
+    <row r="34" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="240"/>
+      <c r="B34" s="241"/>
+      <c r="C34" s="201"/>
+      <c r="D34" s="202"/>
+      <c r="E34" s="211"/>
+      <c r="F34" s="201"/>
+      <c r="G34" s="202"/>
+      <c r="H34" s="211"/>
+    </row>
+    <row r="35" spans="1:8" s="1" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="242"/>
+      <c r="B35" s="243"/>
+      <c r="C35" s="245" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="241"/>
-      <c r="E34" s="242"/>
-      <c r="F34" s="240" t="s">
+      <c r="D35" s="246"/>
+      <c r="E35" s="247"/>
+      <c r="F35" s="245" t="s">
         <v>103</v>
       </c>
-      <c r="G34" s="242"/>
-    </row>
-    <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="225"/>
-      <c r="F35" s="225"/>
-      <c r="G35" s="225"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="G35" s="246"/>
+      <c r="H35" s="247"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="232"/>
+      <c r="F36" s="232"/>
+      <c r="G36" s="232"/>
+      <c r="H36" s="232"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="226"/>
-      <c r="F36" s="226"/>
-      <c r="G36" s="226"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="227" t="s">
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="233"/>
+      <c r="F37" s="233"/>
+      <c r="G37" s="233"/>
+      <c r="H37" s="233"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="234" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="227"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="227" t="s">
+      <c r="B39" s="234"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="234" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="227"/>
+      <c r="B40" s="234"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D7:E7"/>
+  <mergeCells count="64">
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G15:G21"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H15:H21"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:E10"/>
+    <mergeCell ref="F8:G10"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="A27:B27"/>
@@ -5853,18 +5944,30 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:E30"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E37:H37"/>
     <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="A33:B35"/>
     <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
     <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="79" orientation="portrait" r:id="rId1"/>

</xml_diff>